<commit_message>
basic resource system temporarly finished
</commit_message>
<xml_diff>
--- a/data table.xlsx
+++ b/data table.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F957E33-51BB-44EF-927F-8BD3F034737C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B8D697-6E3A-4C20-BD32-8D31258CDC66}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Building" sheetId="1" r:id="rId1"/>
-    <sheet name="Unit" sheetId="2" r:id="rId2"/>
-    <sheet name="Resource" sheetId="3" r:id="rId3"/>
+    <sheet name="Natrual" sheetId="4" r:id="rId2"/>
+    <sheet name="Unit" sheetId="2" r:id="rId3"/>
+    <sheet name="Resource" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,6 +82,34 @@
   </si>
   <si>
     <t>Requests</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Production</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Production</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Consumes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>food</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carrot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -148,13 +177,13 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -436,78 +465,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9" style="3"/>
+    <col min="1" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852F3242-5461-4EAE-942F-C620DCD0D681}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="D1" s="3"/>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3">
-        <v>-1</v>
-      </c>
-      <c r="D3" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>0</v>
       </c>
     </row>
@@ -522,48 +636,57 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A924B124-3095-4D82-A6E6-4F4E795F6422}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" style="3"/>
-    <col min="2" max="2" width="15.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="9" style="2"/>
+    <col min="2" max="2" width="15.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
         <v>1</v>
       </c>
     </row>
@@ -577,7 +700,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B9C121-B123-4CF7-A66D-7F6AD7425759}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -587,66 +710,66 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9" style="3"/>
+    <col min="1" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>2</v>
       </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>